<commit_message>
Fixed: commas in population-->export value as text
</commit_message>
<xml_diff>
--- a/ElectoralData.xlsx
+++ b/ElectoralData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="States-Population-Electoral" sheetId="1" r:id="rId1"/>
@@ -746,14 +746,17 @@
     <t>Population</t>
   </si>
   <si>
-    <t>Electoral Votes</t>
+    <t>ElectoralVotes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -780,6 +783,13 @@
       <color theme="1"/>
       <name val="MS sans serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -904,30 +914,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -946,8 +945,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1259,589 +1271,590 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="10">
         <v>4779736</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="11">
         <v>710231</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="11">
         <v>6392017</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="11">
         <v>2915918</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="11">
         <v>37253956</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="11">
         <v>5029196</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="11">
         <v>3574097</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="11">
         <v>897934</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="11">
         <v>601723</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="11">
         <v>18801310</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="11">
         <v>9687653</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="11">
         <v>1360301</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="11">
         <v>1567582</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="11">
         <v>12830632</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="11">
         <v>6483802</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="11">
         <v>3046355</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="11">
         <v>2853118</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="11">
         <v>4339367</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="11">
         <v>4533372</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="11">
         <v>1328361</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="11">
         <v>5773552</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="11">
         <v>6547629</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="11">
         <v>9883640</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="11">
         <v>5303925</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="11">
         <v>2967297</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="11">
         <v>5988927</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="11">
         <v>989415</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="11">
         <v>1826341</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="11">
         <v>2700551</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="11">
         <v>1316470</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="11">
         <v>8791894</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="11">
         <v>2059179</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="11">
         <v>19378102</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="7">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="11">
         <v>9535483</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="11">
         <v>672591</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="11">
         <v>11536504</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="7">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="11">
         <v>3751351</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="11">
         <v>3831074</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="11">
         <v>12702379</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="11">
         <v>1052567</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="11">
         <v>4625364</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="11">
         <v>814180</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="11">
         <v>6346105</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="11">
         <v>25145561</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="11">
         <v>2763885</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="11">
         <v>625741</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="11">
         <v>8001024</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="11">
         <v>6724540</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="11">
         <v>1852994</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="11">
         <v>5686986</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="12">
         <v>563626</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="8">
         <v>3</v>
       </c>
     </row>

</xml_diff>